<commit_message>
Added min and max purity cases to computeRho.m and implemented a scheme for plotting the coherency matrices onto the Bloch sphere using Stokes parameters
</commit_message>
<xml_diff>
--- a/CP_1.21mW_polarimeter.xlsx
+++ b/CP_1.21mW_polarimeter.xlsx
@@ -16,6 +16,8 @@
     <sheet name="measured" sheetId="1" r:id="rId1"/>
     <sheet name="calculated" sheetId="2" r:id="rId2"/>
     <sheet name="rho_mat" sheetId="3" r:id="rId3"/>
+    <sheet name="rho_min" sheetId="4" r:id="rId7"/>
+    <sheet name="rho_max" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="10">
   <si>
     <t>s0</t>
   </si>
@@ -88,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="226">
     <border>
       <left/>
       <right/>
@@ -125,11 +127,213 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -154,6 +358,208 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="93" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="99" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="101" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="114" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="115" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="116" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="117" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="120" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="121" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="125" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="126" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="131" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="132" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1263,22 +1669,22 @@
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="220" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="220" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="220" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="220" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1307,7 +1713,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.046448475234149973</v>
+        <v>0.046448475234149959</v>
       </c>
       <c r="C3">
         <v>0.95355152476585003</v>
@@ -1330,7 +1736,7 @@
         <v>0.18299262298526431</v>
       </c>
       <c r="C4">
-        <v>0.81700737701473569</v>
+        <v>0.8170073770147358</v>
       </c>
       <c r="D4">
         <v>-0.27185854170345869</v>
@@ -1373,10 +1779,10 @@
         <v>0.53097311618840859</v>
       </c>
       <c r="D6">
-        <v>-0.13156991358567205</v>
+        <v>-0.13156991358567202</v>
       </c>
       <c r="E6">
-        <v>-0.48138344766786312</v>
+        <v>-0.48138344766786306</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1467,7 +1873,7 @@
         <v>90</v>
       </c>
       <c r="B11">
-        <v>0.0046085791735393485</v>
+        <v>0.0046085791735393468</v>
       </c>
       <c r="C11">
         <v>0.9953914208264607</v>
@@ -1487,7 +1893,7 @@
         <v>100</v>
       </c>
       <c r="B12">
-        <v>0.057787635148832735</v>
+        <v>0.057787635148832728</v>
       </c>
       <c r="C12">
         <v>0.94221236485116722</v>
@@ -1513,7 +1919,7 @@
         <v>0.79226354101372398</v>
       </c>
       <c r="D13">
-        <v>-0.29563455791987331</v>
+        <v>-0.29563455791987325</v>
       </c>
       <c r="E13">
         <v>0.27781690105870971</v>
@@ -1533,7 +1939,7 @@
         <v>0.62041340786825849</v>
       </c>
       <c r="D14">
-        <v>-0.27124591275110416</v>
+        <v>-0.27124591275110421</v>
       </c>
       <c r="E14">
         <v>0.40240062848443403</v>
@@ -1665,4 +2071,838 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F20"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" customWidth="true"/>
+    <col min="2" max="2" width="12.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="14.42578125" customWidth="true"/>
+    <col min="5" max="5" width="14.42578125" customWidth="true"/>
+    <col min="6" max="6" width="8.5703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="222" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="222" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="222" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="222" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="222" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="222" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.10751885112282542</v>
+      </c>
+      <c r="C2">
+        <v>0.89248114887717456</v>
+      </c>
+      <c r="D2">
+        <v>-0.010596991019683713</v>
+      </c>
+      <c r="E2">
+        <v>0.047018582003302521</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.13237696944584326</v>
+      </c>
+      <c r="C3">
+        <v>0.86762303055415679</v>
+      </c>
+      <c r="D3">
+        <v>-0.14285830967334529</v>
+      </c>
+      <c r="E3">
+        <v>-0.093219174465882682</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0.24328480732079821</v>
+      </c>
+      <c r="C4">
+        <v>0.75671519267920173</v>
+      </c>
+      <c r="D4">
+        <v>-0.22015329287319579</v>
+      </c>
+      <c r="E4">
+        <v>-0.22265936350511908</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>0.38205654323897253</v>
+      </c>
+      <c r="C5">
+        <v>0.61794345676102747</v>
+      </c>
+      <c r="D5">
+        <v>-0.20432566090514426</v>
+      </c>
+      <c r="E5">
+        <v>-0.32547896278906718</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0.47508718504258246</v>
+      </c>
+      <c r="C6">
+        <v>0.52491281495741748</v>
+      </c>
+      <c r="D6">
+        <v>-0.10582651390917869</v>
+      </c>
+      <c r="E6">
+        <v>-0.3871943876219246</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>0.48375944976013191</v>
+      </c>
+      <c r="C7">
+        <v>0.51624055023986815</v>
+      </c>
+      <c r="D7">
+        <v>0.028141625455643415</v>
+      </c>
+      <c r="E7">
+        <v>-0.39626942585278141</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>0.39936054132861215</v>
+      </c>
+      <c r="C8">
+        <v>0.60063945867138779</v>
+      </c>
+      <c r="D8">
+        <v>0.1370308689327645</v>
+      </c>
+      <c r="E8">
+        <v>-0.36076150209992086</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>0.27635297324174463</v>
+      </c>
+      <c r="C9">
+        <v>0.72364702675825532</v>
+      </c>
+      <c r="D9">
+        <v>0.15694539481340974</v>
+      </c>
+      <c r="E9">
+        <v>-0.28472209584636626</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>0.15863259598023485</v>
+      </c>
+      <c r="C10">
+        <v>0.84136740401976506</v>
+      </c>
+      <c r="D10">
+        <v>0.09755378681666721</v>
+      </c>
+      <c r="E10">
+        <v>-0.17697967630100184</v>
+      </c>
+      <c r="F10">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <v>0.10311053966080717</v>
+      </c>
+      <c r="C11">
+        <v>0.89688946033919281</v>
+      </c>
+      <c r="D11">
+        <v>-0.029276244501280455</v>
+      </c>
+      <c r="E11">
+        <v>-0.045687462349127086</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>0.1412879993239885</v>
+      </c>
+      <c r="C12">
+        <v>0.8587120006760115</v>
+      </c>
+      <c r="D12">
+        <v>-0.16376507238135107</v>
+      </c>
+      <c r="E12">
+        <v>0.094911934360684666</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>110</v>
+      </c>
+      <c r="B13">
+        <v>0.26104696909219521</v>
+      </c>
+      <c r="C13">
+        <v>0.73895303090780473</v>
+      </c>
+      <c r="D13">
+        <v>-0.2417091554116402</v>
+      </c>
+      <c r="E13">
+        <v>0.22714153915719767</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>120</v>
+      </c>
+      <c r="B14">
+        <v>0.40122495728848212</v>
+      </c>
+      <c r="C14">
+        <v>0.59877504271151794</v>
+      </c>
+      <c r="D14">
+        <v>-0.22250285156479652</v>
+      </c>
+      <c r="E14">
+        <v>0.33008898235990136</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>0.4967685669901174</v>
+      </c>
+      <c r="C15">
+        <v>0.5032314330098826</v>
+      </c>
+      <c r="D15">
+        <v>-0.11663903887009502</v>
+      </c>
+      <c r="E15">
+        <v>0.38431314289981888</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <v>0.50325251847504326</v>
+      </c>
+      <c r="C16">
+        <v>0.49674748152495674</v>
+      </c>
+      <c r="D16">
+        <v>0.026739759587709609</v>
+      </c>
+      <c r="E16">
+        <v>0.39626199744679336</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <v>0.42307029927008666</v>
+      </c>
+      <c r="C17">
+        <v>0.57692970072991334</v>
+      </c>
+      <c r="D17">
+        <v>0.13405121152965521</v>
+      </c>
+      <c r="E17">
+        <v>0.36083349310465906</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>160</v>
+      </c>
+      <c r="B18">
+        <v>0.28288374549416007</v>
+      </c>
+      <c r="C18">
+        <v>0.71711625450583993</v>
+      </c>
+      <c r="D18">
+        <v>0.16762541330327385</v>
+      </c>
+      <c r="E18">
+        <v>0.27910288245314552</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>170</v>
+      </c>
+      <c r="B19">
+        <v>0.15823002616890203</v>
+      </c>
+      <c r="C19">
+        <v>0.84176997383109786</v>
+      </c>
+      <c r="D19">
+        <v>0.10678235509483582</v>
+      </c>
+      <c r="E19">
+        <v>0.16994591801548967</v>
+      </c>
+      <c r="F19">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>180</v>
+      </c>
+      <c r="B20">
+        <v>0.10332930312388966</v>
+      </c>
+      <c r="C20">
+        <v>0.89667069687611034</v>
+      </c>
+      <c r="D20">
+        <v>-0.010390213092367789</v>
+      </c>
+      <c r="E20">
+        <v>0.044990134523109786</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F20"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" customWidth="true"/>
+    <col min="2" max="2" width="14.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="14.42578125" customWidth="true"/>
+    <col min="5" max="5" width="14.42578125" customWidth="true"/>
+    <col min="6" max="6" width="8.5703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="224" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="224" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="224" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="224" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="224" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="224" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.0037280465348734876</v>
+      </c>
+      <c r="C2">
+        <v>0.99627195346512643</v>
+      </c>
+      <c r="D2">
+        <v>-0.013399342743558416</v>
+      </c>
+      <c r="E2">
+        <v>0.059452545954612121</v>
+      </c>
+      <c r="F2">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.046448475500789906</v>
+      </c>
+      <c r="C3">
+        <v>0.9535515244992101</v>
+      </c>
+      <c r="D3">
+        <v>-0.17625012242039304</v>
+      </c>
+      <c r="E3">
+        <v>-0.11500829702596792</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0.18299262328529478</v>
+      </c>
+      <c r="C4">
+        <v>0.81700737671470514</v>
+      </c>
+      <c r="D4">
+        <v>-0.27185854144615335</v>
+      </c>
+      <c r="E4">
+        <v>-0.27495318835269816</v>
+      </c>
+      <c r="F4">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>0.35330061352512782</v>
+      </c>
+      <c r="C5">
+        <v>0.64669938647487224</v>
+      </c>
+      <c r="D5">
+        <v>-0.2541425350673801</v>
+      </c>
+      <c r="E5">
+        <v>-0.40483436269277939</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0.46902688382941682</v>
+      </c>
+      <c r="C6">
+        <v>0.53097311617058318</v>
+      </c>
+      <c r="D6">
+        <v>-0.13156991350995073</v>
+      </c>
+      <c r="E6">
+        <v>-0.48138344739083849</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>0.47957673438743614</v>
+      </c>
+      <c r="C7">
+        <v>0.52042326561256391</v>
+      </c>
+      <c r="D7">
+        <v>0.035389434653450638</v>
+      </c>
+      <c r="E7">
+        <v>-0.49832768094655794</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>0.37382737162118568</v>
+      </c>
+      <c r="C8">
+        <v>0.62617262837881427</v>
+      </c>
+      <c r="D8">
+        <v>0.17179687898296683</v>
+      </c>
+      <c r="E8">
+        <v>-0.45229006136116223</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>0.21662222497073449</v>
+      </c>
+      <c r="C9">
+        <v>0.78337777502926553</v>
+      </c>
+      <c r="D9">
+        <v>0.19886173953650388</v>
+      </c>
+      <c r="E9">
+        <v>-0.36076452789075286</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>0.069740237018533768</v>
+      </c>
+      <c r="C10">
+        <v>0.93025976298146629</v>
+      </c>
+      <c r="D10">
+        <v>0.12295687490787335</v>
+      </c>
+      <c r="E10">
+        <v>-0.22306533277968371</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <v>0.0046085796420971816</v>
+      </c>
+      <c r="C11">
+        <v>0.99539142035790285</v>
+      </c>
+      <c r="D11">
+        <v>-0.036542165503310998</v>
+      </c>
+      <c r="E11">
+        <v>-0.057026399356484125</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>0.057787635435619433</v>
+      </c>
+      <c r="C12">
+        <v>0.94221236456438062</v>
+      </c>
+      <c r="D12">
+        <v>-0.20188602487326024</v>
+      </c>
+      <c r="E12">
+        <v>0.11700537155132996</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>110</v>
+      </c>
+      <c r="B13">
+        <v>0.20773645934662813</v>
+      </c>
+      <c r="C13">
+        <v>0.7922635406533719</v>
+      </c>
+      <c r="D13">
+        <v>-0.29563455755536411</v>
+      </c>
+      <c r="E13">
+        <v>0.27781690071616005</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>120</v>
+      </c>
+      <c r="B14">
+        <v>0.37958659224060654</v>
+      </c>
+      <c r="C14">
+        <v>0.62041340775939346</v>
+      </c>
+      <c r="D14">
+        <v>-0.27124591250594798</v>
+      </c>
+      <c r="E14">
+        <v>0.40240062812092575</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>0.495977164927634</v>
+      </c>
+      <c r="C15">
+        <v>0.504022835072366</v>
+      </c>
+      <c r="D15">
+        <v>-0.14520481004516397</v>
+      </c>
+      <c r="E15">
+        <v>0.47843429998406578</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <v>0.50409455060018538</v>
+      </c>
+      <c r="C16">
+        <v>0.49590544939981474</v>
+      </c>
+      <c r="D16">
+        <v>0.03366231414479845</v>
+      </c>
+      <c r="E16">
+        <v>0.49884875733251999</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <v>0.40201070597430849</v>
+      </c>
+      <c r="C17">
+        <v>0.59798929402569156</v>
+      </c>
+      <c r="D17">
+        <v>0.17074788354105627</v>
+      </c>
+      <c r="E17">
+        <v>0.45961207329123593</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>160</v>
+      </c>
+      <c r="B18">
+        <v>0.22258914104271463</v>
+      </c>
+      <c r="C18">
+        <v>0.77741085895728534</v>
+      </c>
+      <c r="D18">
+        <v>0.21417608733794929</v>
+      </c>
+      <c r="E18">
+        <v>0.35661157905935958</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>170</v>
+      </c>
+      <c r="B19">
+        <v>0.068849860138126953</v>
+      </c>
+      <c r="C19">
+        <v>0.93115013986187312</v>
+      </c>
+      <c r="D19">
+        <v>0.13470822734319882</v>
+      </c>
+      <c r="E19">
+        <v>0.21439041440645615</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>180</v>
+      </c>
+      <c r="B20">
+        <v>0.0033534720060074109</v>
+      </c>
+      <c r="C20">
+        <v>0.99664652799399256</v>
+      </c>
+      <c r="D20">
+        <v>-0.013008934862294255</v>
+      </c>
+      <c r="E20">
+        <v>0.056329328787963796</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>